<commit_message>
Update CCDI studies 470, 471
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC01_CCDI_phs000470_Sampleanatomic-C64.9KidneyNOS_Tumorclass-Notappl.xlsx
+++ b/InputFiles/CCDI/TC01_CCDI_phs000470_Sampleanatomic-C64.9KidneyNOS_Tumorclass-Notappl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatekaraa\Automation\03-31-25\Commons_Automation\InputFiles\CCDI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git2/Commons_Automation/InputFiles/CCDI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BBBD30-51C0-4098-9232-8329DA8E5AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE35FC13-B07B-2046-9161-1B557FEC7B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="29380" windowHeight="17360" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -102,136 +102,295 @@
 left join funding f on s.study_id = f.study </t>
   </si>
   <si>
-    <t>with file_data as (
-select file_name, data_category, file_type, file_size, file_access, file_description,"study.id" studyid, "participant.id" as participantid from df_clinical_measure_file )
-SELECT fd.file_name AS "File Name",
-    fd.data_category AS "Data Category",
-    COALESCE(fd.file_description, '') AS "File Description",
-    fd.file_type AS "File Type" ,
-        CASE     
-    WHEN fd.file_size &gt;= 1024 * 1024 * 1024 THEN 
-        CASE 
-            WHEN ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) = CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT) 
-            THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' GB'
-            ELSE ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB'
-        END
-    WHEN fd.file_size &gt;= 1024 * 1024 THEN 
-        CASE 
-            WHEN ROUND(fd.file_size / (1024.0 * 1024.0), 2) = CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT) 
-            THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' MB'
-            ELSE ROUND(fd.file_size / (1024.0 * 1024.0), 2) || ' MB'
-        END
-    WHEN fd.file_size &gt;= 1024 THEN 
-        CASE 
-            WHEN ROUND(fd.file_size / 1024.0, 2) = CAST(ROUND(fd.file_size / 1024.0, 0) AS INT) 
-            THEN CAST(CAST(ROUND(fd.file_size / 1024.0, 0) AS INT) AS TEXT) || ' KB'
-            ELSE ROUND(fd.file_size / 1024.0, 2) || ' KB'
-        END
-    ELSE 
-        CASE 
-            WHEN ROUND(fd.file_size, 2) = CAST(ROUND(fd.file_size, 0) AS INT) 
-            THEN CAST(CAST(ROUND(fd.file_size, 0) AS INT) AS TEXT) || ' Bytes'
-            ELSE ROUND(fd.file_size, 2) || ' Bytes'
-        END
-END AS "File Size",
-fd.file_access AS "File Access", std.dbgap_accession AS "Study ID", fd.participantid AS "Participant ID", null as "Sample ID"
-FROM 
-    df_study std
- LEFT JOIN  
-    file_data fd ON std.id = fd.studyid
-WHERE 
-    std.dbgap_accession = 'phs000470'</t>
-  </si>
-  <si>
     <t>TC01_CCDI_phs000470_Sampleanatomic-C64.9KidneyNOS_Tumorclass-Notappl_TSVData.xlsx</t>
   </si>
   <si>
     <t>TC01_CCDI_phs000470_Sampleanatomic-C64.9KidneyNOS_Tumorclass-Notappl_WebData.xlsx</t>
   </si>
   <si>
-    <t>SELECT DISTINCT
-   smp.sample_id AS "Sample ID",
-    prt.participant_id AS "Participant ID", std.dbgap_accession AS "Study ID" , smp.anatomic_site AS "Sample Anatomic Site", 
-    COALESCE(CASE WHEN smp.participant_age_at_collection = -999 THEN 'Not Reported' ELSE smp.participant_age_at_collection END, 0) AS "Age at Sample Collection (days)",
-    COALESCE(smp.sample_tumor_status, '') AS "Sample Tumor Status",
-    COALESCE(smp.tumor_classification, '') AS "Sample Tumor Classification",
- dgn.diagnosis as "Sample Diagnosis"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_sample smp ON prt.id = smp."participant.id"
-LEFT JOIN 
-    df_diagnosis dgn ON smp."id" = dgn."sample.id"
-WHERE 
-   std.dbgap_accession = 'phs000470' and  smp.anatomic_site = 'C64.9 : Kidney, NOS' and smp.tumor_classification = 'Not Applicable'
-AND smp.sample_id IS NOT NULL
-ORDER BY 
-   smp.sample_id ASC
-;</t>
-  </si>
-  <si>
-    <t>with diagnosis1 as (
-select dgn."participant.id", group_concat(dgn.age_at_diagnosis,';') as age, group_concat(dgn.diagnosis,';') as diag,group_concat(dgn.anatomic_site,';') as ant_site from df_diagnosis dgn where dgn."participant.id" is not null group by dgn."participant.id" ),
-diagnosis2 as (select "participant.id",  group_concat(diagnosis,';') as diag from (select distinct "participant.id", diagnosis from df_diagnosis  where "participant.id" is not null )  group by "participant.id" ),
-diagnosis3 as (select "participant.id",  group_concat(anatomic_site,';') as ant_site from (select distinct "participant.id", anatomic_site from df_diagnosis where "participant.id" is not null ) group by "participant.id" ) 
+    <t>WITH diagnosis_age AS (
+  SELECT
+    d."participant.id",
+    GROUP_CONCAT(
+      CASE
+        WHEN COALESCE(CAST(d.age_at_diagnosis AS TEXT), '') IN ('', '-999') THEN 'Not Reported'
+        ELSE CAST(d.age_at_diagnosis AS TEXT)
+      END,
+      ';'
+    ) AS age_days
+  FROM df_diagnosis d
+  WHERE d."participant.id" IS NOT NULL
+  GROUP BY d."participant.id"
+),
+diagnosis_list AS (
+  SELECT t."participant.id",
+         GROUP_CONCAT(t.diagnosis, ';') AS diag
+  FROM (
+    SELECT DISTINCT "participant.id", COALESCE(diagnosis, '') AS diagnosis
+    FROM df_diagnosis
+    WHERE "participant.id" IS NOT NULL
+  ) t
+  GROUP BY t."participant.id"
+),
+anatomic_list AS (
+  SELECT t."participant.id",
+         GROUP_CONCAT(t.anatomic_site, ';') AS ant_site
+  FROM (
+    SELECT DISTINCT "participant.id", COALESCE(anatomic_site, '') AS anatomic_site
+    FROM df_diagnosis
+    WHERE "participant.id" IS NOT NULL
+  ) t
+  GROUP BY t."participant.id"
+),
+category_list AS (
+  SELECT t."participant.id",
+         GROUP_CONCAT(t.diagnosis_category, ';') AS diag_cat
+  FROM (
+    SELECT DISTINCT "participant.id", COALESCE(diagnosis_category, '') AS diagnosis_category
+    FROM df_diagnosis
+    WHERE "participant.id" IS NOT NULL
+  ) t
+  GROUP BY t."participant.id"
+),
+scope_participants AS (
+  SELECT DISTINCT prt.id AS participant_row_id
+  FROM df_participant prt
+  LEFT JOIN df_consent_group cg ON prt."consent_group.id" = cg.id
+  LEFT JOIN df_study std        ON cg."study.id" = std.id
+  LEFT JOIN df_sample smp       ON prt.id = smp."participant.id"
+  WHERE std.dbgap_accession = 'phs000470'
+    AND smp.anatomic_site = 'C64.9 : Kidney, NOS'
+    AND smp.tumor_classification = 'Not Applicable'
+)
 SELECT DISTINCT
-    prt.participant_id AS "Participant ID",
-    std.dbgap_accession AS "Study ID",
-    COALESCE(prt.sex_at_birth, '') AS "Sex",
-    COALESCE(prt.race, '') AS "Race",
-	dgn2.diag AS "Diagnosis",
-	dgn3.ant_site AS "Diagnosis Anatomic Site",
-	   COALESCE(CASE WHEN dgn1.age = '-999' THEN 'Not Reported' ELSE dgn1.age END, "") AS "Age at Diagnosis (days)",
-	null AS "Treatment Type",
-	srv.last_known_survival_status AS "Last Known Survival Status"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    diagnosis1 dgn1 ON prt.id = dgn1."participant.id" 
-LEFT JOIN 
-    diagnosis2 dgn2 ON prt.id = dgn2."participant.id"
-LEFT JOIN 
-    diagnosis3 dgn3 ON prt.id = dgn3."participant.id"
-LEFT JOIN 
-    df_survival srv ON prt.id = srv."participant.id"
-LEFT JOIN 
-    df_sample smp ON prt.id = smp."participant.id"
-WHERE 
-     std.dbgap_accession = 'phs000470' and  smp.anatomic_site = 'C64.9 : Kidney, NOS' and smp.tumor_classification = 'Not Applicable'
-ORDER BY 
-    prt.participant_id ASC 
-Limit 100
-;</t>
-  </si>
-  <si>
-    <t>SELECT
-    COUNT(DISTINCT std.dbgap_accession) AS "Studies",
-    COUNT(DISTINCT prt.participant_id) AS "Participants",
-    COUNT(DISTINCT smp.sample_id) AS "Samples",
-    (COUNT(DISTINCT cmf.id)) AS "Files"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_sample smp ON prt.id = smp."participant.id"
-LEFT JOIN 
-    df_clinical_measure_file cmf ON std.id = cmf."study.id"
-WHERE 
-     std.dbgap_accession = 'phs000470' and  smp.anatomic_site = 'C64.9 : Kidney, NOS' and smp.tumor_classification = 'Not Applicable';</t>
+  prt.participant_id                          AS "Participant ID",
+  std.dbgap_accession                         AS "Study ID",
+  COALESCE(prt.sex_at_birth, '')              AS "Sex",
+  COALESCE(prt.race, '')                      AS "Race",
+  COALESCE(dl.diag, '')                       AS "Diagnosis",
+  COALESCE(al.ant_site, '')                   AS "Diagnosis Anatomic Site",
+  COALESCE(cl.diag_cat, '')                   AS "Diagnosis Category",
+  COALESCE(da.age_days, '')                   AS "Age at Diagnosis (days)",
+  NULL                                        AS "Treatment Type",
+  COALESCE(srv.last_known_survival_status,'') AS "Last Known Survival Status"
+FROM scope_participants sp
+JOIN df_participant prt      ON prt.id = sp.participant_row_id
+LEFT JOIN df_consent_group cg ON prt."consent_group.id" = cg.id
+LEFT JOIN df_study std        ON cg."study.id" = std.id
+LEFT JOIN diagnosis_age da    ON prt.id = da."participant.id"
+LEFT JOIN diagnosis_list dl   ON prt.id = dl."participant.id"
+LEFT JOIN anatomic_list al    ON prt.id = al."participant.id"
+LEFT JOIN category_list cl    ON prt.id = cl."participant.id"
+LEFT JOIN df_survival srv     ON prt.id = srv."participant.id"
+ORDER BY prt.participant_id ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>WITH scope_participants AS (
+  SELECT DISTINCT prt.id AS participant_row_id
+  FROM df_participant prt
+  LEFT JOIN df_consent_group cg ON prt."consent_group.id" = cg.id
+  LEFT JOIN df_study std        ON cg."study.id" = std.id
+  LEFT JOIN df_sample smp       ON prt.id = smp."participant.id"
+  WHERE std.dbgap_accession = 'phs000470'
+    AND smp.anatomic_site = 'C64.9 : Kidney, NOS'
+    AND smp.tumor_classification = 'Not Applicable'
+),
+file_data AS (
+  SELECT
+    cmf.id                                                   AS file_row_id,
+    cmf.file_name,
+    REPLACE(COALESCE(cmf.data_category, ''), ';', ', ')      AS data_category,
+    COALESCE(cmf.file_description, '')                       AS file_description,
+    COALESCE(cmf.file_type, '')                              AS file_type,
+    COALESCE(cmf.file_access, '')                            AS file_access,
+    COALESCE(CAST(cmf.file_size AS INTEGER), 0)              AS file_size,
+    cmf."study.id"                                           AS study_row_id,
+    cmf."participant.id"                                     AS participant_row_id,
+    COALESCE(cmf.file_mapping_level, '')                     AS file_mapping_level
+  FROM df_clinical_measure_file cmf
+),
+file_scope AS (
+  SELECT DISTINCT fd.file_row_id
+  FROM file_data fd
+  LEFT JOIN df_study std ON fd.study_row_id = std.id
+  LEFT JOIN scope_participants sp ON fd.participant_row_id = sp.participant_row_id
+  WHERE (std.dbgap_accession = 'phs000470' AND fd.file_mapping_level = 'Study')
+     OR (sp.participant_row_id IS NOT NULL)
+),
+sample_ids_per_file AS (
+  SELECT t.file_row_id,
+         GROUP_CONCAT(t.sample_id, ';') AS sample_ids
+  FROM (
+    SELECT DISTINCT fd.file_row_id, COALESCE(smp.sample_id, '') AS sample_id
+    FROM file_data fd
+    LEFT JOIN df_participant prt ON fd.participant_row_id = prt.id
+    LEFT JOIN df_sample smp ON prt.id = smp."participant.id"
+  ) t
+  GROUP BY t.file_row_id
+),
+study_and_participant AS (
+  SELECT fd.file_row_id,
+         std.dbgap_accession AS study_id,
+         prt.participant_id  AS participant_id
+  FROM file_data fd
+  LEFT JOIN df_study std ON fd.study_row_id = std.id
+  LEFT JOIN df_participant prt ON fd.participant_row_id = prt.id
+)
+SELECT DISTINCT
+  fd.file_name                                     AS "File Name",
+  fd.data_category                                 AS "Data Category",
+  fd.file_description                              AS "File Description",
+  fd.file_type                                     AS "File Type",
+  CASE
+    WHEN fd.file_size &gt;= 1024*1024*1024 THEN
+      CASE WHEN ROUND(fd.file_size / (1024.0*1024*1024), 2) = CAST(ROUND(fd.file_size / (1024.0*1024*1024), 0) AS REAL)
+           THEN CAST(ROUND(fd.file_size / (1024.0*1024*1024), 0) AS TEXT) || ' GB'
+           ELSE CAST(ROUND(fd.file_size / (1024.0*1024*1024), 2) AS TEXT) || ' GB'
+      END
+    WHEN fd.file_size &gt;= 1024*1024 THEN
+      CASE WHEN ROUND(fd.file_size / (1024.0*1024), 2) = CAST(ROUND(fd.file_size / (1024.0*1024), 0) AS REAL)
+           THEN CAST(ROUND(fd.file_size / (1024.0*1024), 0) AS TEXT) || ' MB'
+           ELSE CAST(ROUND(fd.file_size / (1024.0*1024), 2) AS TEXT) || ' MB'
+      END
+    WHEN fd.file_size &gt;= 1024 THEN
+      CASE WHEN ROUND(fd.file_size / 1024.0, 2) = CAST(ROUND(fd.file_size / 1024.0, 0) AS REAL)
+           THEN CAST(ROUND(fd.file_size / 1024.0, 0) AS TEXT) || ' KB'
+           ELSE CAST(ROUND(fd.file_size / 1024.0, 2) AS TEXT) || ' KB'
+      END
+    ELSE CAST(fd.file_size AS TEXT)
+  END                                              AS "File Size",
+  fd.file_access                                   AS "Access",
+  sap.study_id                                     AS "Study ID",
+  COALESCE(sap.participant_id, '')                 AS "Participant ID",
+  COALESCE(sif.sample_ids, '')                     AS "Sample ID"
+FROM file_scope fs
+JOIN file_data fd                  ON fd.file_row_id = fs.file_row_id
+LEFT JOIN study_and_participant sap ON fd.file_row_id = sap.file_row_id
+LEFT JOIN sample_ids_per_file sif   ON fd.file_row_id = sif.file_row_id
+ORDER BY fd.file_name ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>WITH scope_participants AS (
+  -- participants that satisfy study + sample filters
+  SELECT DISTINCT prt.id AS participant_row_id
+  FROM df_participant prt
+  LEFT JOIN df_consent_group cg ON prt."consent_group.id" = cg.id
+  LEFT JOIN df_study std        ON cg."study.id" = std.id
+  LEFT JOIN df_sample smp       ON prt.id = smp."participant.id"
+  WHERE std.dbgap_accession = 'phs000470'
+    AND smp.anatomic_site = 'C64.9 : Kidney, NOS'
+    AND smp.tumor_classification = 'Not Applicable'
+),
+scope_samples AS (
+  -- ONLY samples that themselves match the filters (not all samples of those participants)
+  SELECT DISTINCT smp.id AS sample_row_id
+  FROM df_sample smp
+  JOIN df_participant prt  ON smp."participant.id" = prt.id
+  LEFT JOIN df_consent_group cg ON prt."consent_group.id" = cg.id
+  LEFT JOIN df_study std        ON cg."study.id" = std.id
+  WHERE std.dbgap_accession = 'phs000470'
+    AND smp.anatomic_site = 'C64.9 : Kidney, NOS'
+    AND smp.tumor_classification = 'Not Applicable'
+    -- (optional) also ensure the participant itself is in scope (redundant but safe)
+    AND prt.id IN (SELECT participant_row_id FROM scope_participants)
+),
+scope_files AS (
+  -- files linked to scoped participants OR study-level files for phs000470
+  SELECT DISTINCT fd.id AS file_row_id
+  FROM df_clinical_measure_file fd
+  LEFT JOIN df_study std ON fd."study.id" = std.id
+  WHERE (COALESCE(fd."participant.id",'') IN (
+           SELECT CAST(participant_row_id AS TEXT) FROM scope_participants
+        ))
+     OR (std.dbgap_accession = 'phs000470' AND COALESCE(fd.file_mapping_level,'') = 'Study')
+)
+SELECT
+  (SELECT COUNT(DISTINCT std.dbgap_accession)
+     FROM df_study std
+     WHERE std.dbgap_accession = 'phs000470')   AS "Studies Count",
+  (SELECT COUNT(DISTINCT sp.participant_row_id)
+     FROM scope_participants sp)                AS "Participants Count",
+  (SELECT COUNT(DISTINCT ss.sample_row_id)
+     FROM scope_samples ss)                     AS "Samples Count",
+  (SELECT COUNT(DISTINCT sf.file_row_id)
+     FROM scope_files sf)                       AS "Files Count";</t>
+  </si>
+  <si>
+    <t>WITH scope_samples AS (
+  -- Only samples that themselves match the TC01 filters
+  SELECT DISTINCT smp.id AS sample_row_id
+  FROM df_sample smp
+  JOIN df_participant prt   ON smp."participant.id" = prt.id
+  LEFT JOIN df_consent_group cg ON prt."consent_group.id" = cg.id
+  LEFT JOIN df_study std        ON cg."study.id" = std.id
+  WHERE std.dbgap_accession = 'phs000470'
+    AND smp.anatomic_site = 'C64.9 : Kidney, NOS'
+    AND smp.tumor_classification = 'Not Applicable'
+),
+diag_by_sample AS (
+  -- DISTINCT first, then group_concat
+  SELECT t.sample_row_id,
+         GROUP_CONCAT(t.diagnosis, ';')          AS diagnosis_list,
+         GROUP_CONCAT(t.diagnosis_category, ';') AS diagnosis_category_list
+  FROM (
+    SELECT DISTINCT
+      d."sample.id" AS sample_row_id,
+      COALESCE(d.diagnosis, '')          AS diagnosis,
+      COALESCE(d.diagnosis_category, '') AS diagnosis_category
+    FROM df_diagnosis d
+    WHERE d."sample.id" IS NOT NULL
+  ) t
+  GROUP BY t.sample_row_id
+),
+study_for_sample AS (
+  -- Resolve Study ID through participant → consent_group → study
+  SELECT
+    smp.id              AS sample_row_id,
+    std.dbgap_accession AS study_id,
+    prt.participant_id  AS participant_id
+  FROM df_sample smp
+  JOIN df_participant prt   ON smp."participant.id" = prt.id
+  LEFT JOIN df_consent_group cg ON prt."consent_group.id" = cg.id
+  LEFT JOIN df_study std        ON cg."study.id" = std.id
+)
+SELECT DISTINCT
+  smp.sample_id                                      AS "Sample ID",
+  sfs.participant_id                                 AS "Participant ID",
+  sfs.study_id                                       AS "Study ID",
+  COALESCE(smp.anatomic_site, '')                    AS "Sample Anatomic Site",
+  CASE
+    WHEN COALESCE(CAST(smp.participant_age_at_collection AS TEXT), '') IN ('', '-999')
+      THEN 'Not Reported'
+    ELSE CAST(smp.participant_age_at_collection AS TEXT)
+  END                                                AS "Age at Sample Collection (days)",
+  COALESCE(smp.sample_tumor_status, '')             AS "Sample Tumor Status",
+  COALESCE(smp.tumor_classification, '')            AS "Sample Tumor Classification",
+  COALESCE(dbs.diagnosis_list, '')                  AS "Sample Diagnosis",
+  COALESCE(dbs.diagnosis_category_list, '')         AS "Diagnosis Category"
+FROM scope_samples ss
+JOIN df_sample smp             ON smp.id = ss.sample_row_id
+LEFT JOIN study_for_sample sfs ON smp.id = sfs.sample_row_id
+LEFT JOIN diag_by_sample dbs   ON smp.id = dbs.sample_row_id
+ORDER BY smp.sample_id ASC
+LIMIT 100;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -291,14 +450,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -624,19 +786,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.85546875" customWidth="1"/>
-    <col min="4" max="4" width="70.140625" customWidth="1"/>
-    <col min="5" max="5" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.83203125" customWidth="1"/>
+    <col min="4" max="4" width="70.1640625" customWidth="1"/>
+    <col min="5" max="5" width="63.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -653,24 +815,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -679,33 +841,33 @@
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="393.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>13</v>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>10</v>
+      <c r="B5" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C7" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>